<commit_message>
Uploaded BC, Exibits and PC #37
</commit_message>
<xml_diff>
--- a/Documents/Management/ManagementDocs/Iniziation/C11_Exibits.xlsx
+++ b/Documents/Management/ManagementDocs/Iniziation/C11_Exibits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdell\projects\UniRentHub\Documents\Management\ManagementDocs\Iniziation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisalerno-my.sharepoint.com/personal/r_iuliano13_studenti_unisa_it/Documents/GPS_Documents/ProjectManagerDocuments/Iniziation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0F14031-5636-4D3A-9429-FF2965E11440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="101_{B14786DC-0F51-49F6-A6DB-B7227F0A8A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CD66DB2-E67F-4A88-BBBF-D8301F8EA300}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exibit" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>Date:</t>
   </si>
@@ -87,36 +87,15 @@
     <t>https://colab.research.google.com/signup</t>
   </si>
   <si>
-    <t>Screen telefono</t>
-  </si>
-  <si>
     <t>Manutenzione</t>
   </si>
   <si>
-    <t>https://it.talent.com/salary?job=project+manager</t>
-  </si>
-  <si>
-    <t>Stipendi TMs</t>
-  </si>
-  <si>
-    <t>Stipendi PMs</t>
-  </si>
-  <si>
     <t>Pubblicità IG</t>
   </si>
   <si>
     <t>https://www.hostinger.com/tutorials/website-maintenance-cost</t>
   </si>
   <si>
-    <t>1500 per month</t>
-  </si>
-  <si>
-    <t>https://www.glassdoor.it/Stipendi/software-engineer-stipendio-SRCH_KO0,17.htm</t>
-  </si>
-  <si>
-    <t>https://www.jobbydoo.it/stipendio/software-engineer</t>
-  </si>
-  <si>
     <t>Colab Pro +</t>
   </si>
   <si>
@@ -129,16 +108,10 @@
     <t>https://www.microsoft.com/en-us/sql-server/sql-server-2022-pricing</t>
   </si>
   <si>
-    <t>standard server</t>
-  </si>
-  <si>
     <t>Web Server</t>
   </si>
   <si>
     <t>https://azure.microsoft.com/en-us/pricing/details/app-service/windows/</t>
-  </si>
-  <si>
-    <t>premium</t>
   </si>
   <si>
     <t>Assume the project is completed in
@@ -151,9 +124,6 @@
     <t>https://www.studenti.it/affitti-studenti-fuori-sede-costi.html#:~:text=Affitti%20per%20studenti%3A%20il%20prezzo%20dipende%20dalla%20citt%C3%A0,-Secondo%20il%20centro&amp;text=Nella%20Capitale%2C%20infatti%2C%20per%20una,quinta%20posizione%20con%20447%20euro.</t>
   </si>
   <si>
-    <t>Payback in Year 1</t>
-  </si>
-  <si>
     <t>https://www.glassdoor.it/Stipendi/web-developer-stipendio-SRCH_KO0,13.htm</t>
   </si>
   <si>
@@ -203,9 +173,6 @@
   </si>
   <si>
     <t>Instagram advertisement (euro/days)</t>
-  </si>
-  <si>
-    <t>Maintenance (euro/month)</t>
   </si>
   <si>
     <t>First year</t>
@@ -269,10 +236,40 @@
     <t>Home checker</t>
   </si>
   <si>
-    <t>Stipendi HCs</t>
-  </si>
-  <si>
     <t>Pubblicità TikTok</t>
+  </si>
+  <si>
+    <t>Corrective maintenance (euro)</t>
+  </si>
+  <si>
+    <t>Stipendi PM</t>
+  </si>
+  <si>
+    <t>Stipendi TM</t>
+  </si>
+  <si>
+    <t>Stipendi HC</t>
+  </si>
+  <si>
+    <t>Elemento</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>TikTok</t>
+  </si>
+  <si>
+    <t>https://it.talent.com/salary?job=project+manager+it</t>
+  </si>
+  <si>
+    <t>Immagine</t>
+  </si>
+  <si>
+    <t>Payback in Year 1</t>
   </si>
 </sst>
 </file>
@@ -284,7 +281,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -343,6 +340,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -368,7 +377,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,7 +402,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,6 +419,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -432,7 +449,10 @@
     <cellStyle name="Percentuale" xfId="3" builtinId="5"/>
     <cellStyle name="Valuta" xfId="2" builtinId="4"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -639,19 +659,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>1344930</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1344930</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>146685</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1045" name="Line 3">
+        <xdr:cNvPr id="2" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
@@ -664,8 +684,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="3590925" y="3438525"/>
-          <a:ext cx="0" cy="285750"/>
+          <a:off x="5621655" y="3198495"/>
+          <a:ext cx="0" cy="291465"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -733,20 +753,125 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2095501</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4498835</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>108584</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Immagine 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{404D3F31-A2E6-A776-F3E4-4CD24BF8253F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3992881" y="4686300"/>
+          <a:ext cx="2403334" cy="5206364"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5755006</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9486</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>535305</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>106679</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Immagine 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F39EF30B-45D7-D420-F802-BD7CE58B58D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7652386" y="4611966"/>
+          <a:ext cx="2371724" cy="5278793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA87A7E9-7DFD-4020-A270-1065BD2F57E8}" name="Tabella1" displayName="Tabella1" ref="A23:F26" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA87A7E9-7DFD-4020-A270-1065BD2F57E8}" name="Tabella1" displayName="Tabella1" ref="A23:F26" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A23:F26" xr:uid="{EA87A7E9-7DFD-4020-A270-1065BD2F57E8}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8BA09593-D93E-497F-88FE-1C6F2FF17D9C}" name="Cost" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{61331D10-CF2B-44D5-894E-3FB1ABEEFEF2}" name="People" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{7DBEEF48-AA27-47B7-AB03-CFE6B3C764BA}" name="Hourly wage" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{F5166F56-AC68-463A-ACD8-F7359DD36B3A}" name="Hours per month" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{8BA09593-D93E-497F-88FE-1C6F2FF17D9C}" name="Cost" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{61331D10-CF2B-44D5-894E-3FB1ABEEFEF2}" name="People" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{7DBEEF48-AA27-47B7-AB03-CFE6B3C764BA}" name="Hourly wage" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{F5166F56-AC68-463A-ACD8-F7359DD36B3A}" name="Hours per month" dataDxfId="23">
       <calculatedColumnFormula>PRODUCT(8,5,4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{82315B77-4E44-4E44-96F2-404661125470}" name="Monthly salary" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{82315B77-4E44-4E44-96F2-404661125470}" name="Monthly salary" dataDxfId="22">
       <calculatedColumnFormula>PRODUCT(C24,D24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CA830B4C-D477-40A3-B4AC-D2DB7D7BD96B}" name="Total salary" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{CA830B4C-D477-40A3-B4AC-D2DB7D7BD96B}" name="Total salary" dataDxfId="21">
       <calculatedColumnFormula>PRODUCT(PRODUCT(Tabella1[[#This Row],[Monthly salary]],12),Tabella1[[#This Row],[People]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -755,28 +880,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10A166C8-83BB-4D0D-BD8D-027A08DF4A42}" name="Tabella2" displayName="Tabella2" ref="A28:C37" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{10A166C8-83BB-4D0D-BD8D-027A08DF4A42}" name="Tabella2" displayName="Tabella2" ref="A28:C37" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A28:C37" xr:uid="{10A166C8-83BB-4D0D-BD8D-027A08DF4A42}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{441C5D47-F572-4A6D-8892-68F953A6752F}" name="Cost" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{D89530A7-38D8-441A-8BDB-7FD882211581}" name="Price" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{9D911918-A806-4249-B0CA-38198ACD0462}" name="Total cost" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{441C5D47-F572-4A6D-8892-68F953A6752F}" name="Cost" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{D89530A7-38D8-441A-8BDB-7FD882211581}" name="Price" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{9D911918-A806-4249-B0CA-38198ACD0462}" name="Total cost" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DD2EDE0A-F97B-45E0-B0AD-F537274B5522}" name="Tabella4" displayName="Tabella4" ref="D31:F36" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="D31:F36" xr:uid="{DD2EDE0A-F97B-45E0-B0AD-F537274B5522}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DD2EDE0A-F97B-45E0-B0AD-F537274B5522}" name="Tabella4" displayName="Tabella4" ref="D31:F37" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="D31:F37" xr:uid="{DD2EDE0A-F97B-45E0-B0AD-F537274B5522}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1320C714-27F9-4DAB-9FD8-7E9BF6A153B7}" name="First year" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{1320C714-27F9-4DAB-9FD8-7E9BF6A153B7}" name="First year" dataDxfId="13">
       <calculatedColumnFormula>PRODUCT(Tabella2[[#This Row],[Price]],30,3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{72B7F8C6-D8EB-4ED4-840A-D9CD11A8857A}" name="Second year" dataDxfId="11">
+    <tableColumn id="2" xr3:uid="{72B7F8C6-D8EB-4ED4-840A-D9CD11A8857A}" name="Second year" dataDxfId="12">
       <calculatedColumnFormula>PRODUCT(Tabella2[[#This Row],[Price]],30,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{980705E8-C19F-428B-93D0-EE4EA23CB0B2}" name="Third year" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{980705E8-C19F-428B-93D0-EE4EA23CB0B2}" name="Third year" dataDxfId="11">
       <calculatedColumnFormula>PRODUCT(Tabella2[[#This Row],[Price]],30)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -785,16 +910,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4042F39B-B476-40FF-A245-025F1F7B3466}" name="Tabella46" displayName="Tabella46" ref="D44:F45" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4042F39B-B476-40FF-A245-025F1F7B3466}" name="Tabella46" displayName="Tabella46" ref="D44:F45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="D44:F45" xr:uid="{4042F39B-B476-40FF-A245-025F1F7B3466}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5200E886-1F74-449D-A606-A3927563D96B}" name="First year" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{5200E886-1F74-449D-A606-A3927563D96B}" name="First year" dataDxfId="8">
       <calculatedColumnFormula>PRODUCT(Tabella6[[#This Row],[Price]],0.05,12000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{922784AF-0ACA-41CC-ACAE-6C96734FC0EE}" name="Second year" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{922784AF-0ACA-41CC-ACAE-6C96734FC0EE}" name="Second year" dataDxfId="7">
       <calculatedColumnFormula>PRODUCT(Tabella6[[#This Row],[Price]],0.05,24000)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F2BE196B-547B-4D59-8E50-1E41F3907E1B}" name="Third year" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{F2BE196B-547B-4D59-8E50-1E41F3907E1B}" name="Third year" dataDxfId="6">
       <calculatedColumnFormula>PRODUCT(Tabella6[[#This Row],[Price]],0.05,36000)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -803,12 +928,23 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA8FEF43-E6BE-47B6-8840-D26FCD1DE78E}" name="Tabella6" displayName="Tabella6" ref="A42:C45" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AA8FEF43-E6BE-47B6-8840-D26FCD1DE78E}" name="Tabella6" displayName="Tabella6" ref="A42:C45" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A42:C45" xr:uid="{AA8FEF43-E6BE-47B6-8840-D26FCD1DE78E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D30A4F11-9B21-4A79-A5AC-5DEBD1CE5D1D}" name="Benefits" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{83CB6D05-B386-4183-860C-24A9F6535DAB}" name="Price" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{BE9B4279-979E-4310-99B9-70474AC9D433}" name="Monthly subscription" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D30A4F11-9B21-4A79-A5AC-5DEBD1CE5D1D}" name="Benefits" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{83CB6D05-B386-4183-860C-24A9F6535DAB}" name="Price" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{BE9B4279-979E-4310-99B9-70474AC9D433}" name="Monthly subscription" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C95402A1-1280-456A-963C-2D879391D9B1}" name="Tabella3" displayName="Tabella3" ref="A5:B19" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A5:B19" xr:uid="{C95402A1-1280-456A-963C-2D879391D9B1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9AB3CE7C-D704-43A6-A994-B716DBB9AC62}" name="Elemento"/>
+    <tableColumn id="2" xr3:uid="{6052FFE0-D8FC-45EC-ACF1-C8ABB4DE453D}" name="Link" dataCellStyle="Collegamento ipertestuale"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1167,8 +1303,8 @@
   </sheetPr>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1188,30 +1324,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="A1" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="29"/>
+      <c r="A2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="33"/>
       <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="30">
-        <v>45230</v>
-      </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="D2" s="34">
+        <v>45300</v>
+      </c>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -1236,7 +1372,7 @@
     </row>
     <row r="6" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -1266,19 +1402,19 @@
       </c>
       <c r="B8" s="17">
         <f>SUM(F24:F25,C29:C31)</f>
-        <v>246376.44</v>
+        <v>190372.44</v>
       </c>
       <c r="C8" s="17">
-        <f>SUM(F26,C29:C30,Tabella4[First year],C37)</f>
-        <v>126051</v>
+        <f>SUM(F26,C29:C30,Tabella4[First year])</f>
+        <v>197091</v>
       </c>
       <c r="D8" s="17">
-        <f>SUM(F26,C29:C30,Tabella4[Second year],C37)</f>
-        <v>122021</v>
+        <f>SUM(F26,C29:C30,Tabella4[Second year])</f>
+        <v>185061</v>
       </c>
       <c r="E8" s="17">
-        <f>SUM(F26,C29:C30,Tabella4[Third year],C37)</f>
-        <v>117991</v>
+        <f>SUM(F26,C29:C30,Tabella4[Third year])</f>
+        <v>173031</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1308,23 +1444,23 @@
       </c>
       <c r="B10" s="3">
         <f>B8*B9</f>
-        <v>246376.44</v>
+        <v>190372.44</v>
       </c>
       <c r="C10" s="3">
         <f>C8*C9</f>
-        <v>117227.43000000001</v>
+        <v>183294.63</v>
       </c>
       <c r="D10" s="3">
         <f>D8*D9</f>
-        <v>104938.06</v>
+        <v>159152.46</v>
       </c>
       <c r="E10" s="3">
         <f>E8*E9</f>
-        <v>93212.89</v>
+        <v>136694.49000000002</v>
       </c>
       <c r="F10" s="4">
         <f>SUM(B10:E10)</f>
-        <v>561754.81999999995</v>
+        <v>669514.02</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1399,23 +1535,23 @@
       </c>
       <c r="B16" s="1">
         <f>B14-B10</f>
-        <v>-246376.44</v>
+        <v>-190372.44</v>
       </c>
       <c r="C16" s="1">
         <f>C14-C10</f>
-        <v>258864.57000000007</v>
+        <v>192797.37000000005</v>
       </c>
       <c r="D16" s="1">
         <f>D14-D10</f>
-        <v>590629.94000000018</v>
+        <v>536415.54000000015</v>
       </c>
       <c r="E16" s="1">
         <f>E14-E10</f>
-        <v>865215.11</v>
+        <v>821733.51</v>
       </c>
       <c r="F16" s="4">
         <f>F14-F10</f>
-        <v>1468333.1800000002</v>
+        <v>1360573.9800000002</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>10</v>
@@ -1427,19 +1563,19 @@
       </c>
       <c r="B17" s="1">
         <f>B16</f>
-        <v>-246376.44</v>
+        <v>-190372.44</v>
       </c>
       <c r="C17" s="1">
         <f>B17+C16</f>
-        <v>12488.130000000063</v>
+        <v>2424.9300000000512</v>
       </c>
       <c r="D17" s="1">
         <f>C17+D16</f>
-        <v>603118.0700000003</v>
+        <v>538840.4700000002</v>
       </c>
       <c r="E17" s="9">
         <f>D17+E16</f>
-        <v>1468333.1800000002</v>
+        <v>1360573.9800000002</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1448,281 +1584,290 @@
       </c>
       <c r="B19" s="7">
         <f>(F14-F10)/F10</f>
-        <v>2.6138328105489159</v>
+        <v>2.0321814620103105</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="B20" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>42</v>
+      <c r="A23" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="23">
+      <c r="A24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="22">
         <v>2</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="22">
         <v>24</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="22">
         <f>PRODUCT(8,5,4)</f>
         <v>160</v>
       </c>
-      <c r="E24" s="23">
-        <f t="shared" ref="E24:E25" si="0">PRODUCT(C24,D24)</f>
+      <c r="E24" s="22">
+        <f t="shared" ref="E24" si="0">PRODUCT(C24,D24)</f>
         <v>3840</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="22">
         <f>PRODUCT(PRODUCT(Tabella1[[#This Row],[Monthly salary]],12),Tabella1[[#This Row],[People]])</f>
         <v>92160</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="23">
+      <c r="A25" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="22">
         <v>6</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="22">
         <v>13</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="22">
         <f>PRODUCT(8,5,4)</f>
         <v>160</v>
       </c>
-      <c r="E25" s="23">
-        <f t="shared" si="0"/>
+      <c r="E25" s="22">
+        <f>PRODUCT(C25,D25)</f>
         <v>2080</v>
       </c>
-      <c r="F25" s="23">
-        <f>PRODUCT(PRODUCT(Tabella1[[#This Row],[Monthly salary]],12),Tabella1[[#This Row],[People]])</f>
-        <v>149760</v>
+      <c r="F25" s="22">
+        <f>PRODUCT(SUM(PRODUCT(50,Tabella1[[#This Row],[Hourly wage]]),PRODUCT(Tabella1[[#This Row],[Monthly salary]],0.8,9)),Tabella1[[#This Row],[People]])</f>
+        <v>93756</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="23">
-        <v>6</v>
-      </c>
-      <c r="C26" s="23">
+      <c r="A26" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="22">
+        <v>15</v>
+      </c>
+      <c r="C26" s="22">
         <v>11</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="22">
         <f>PRODUCT(4,5,4)</f>
         <v>80</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="22">
         <f>PRODUCT(C26,D26)</f>
         <v>880</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="22">
         <f>PRODUCT(PRODUCT(Tabella1[[#This Row],[Monthly salary]],12),Tabella1[[#This Row],[People]])</f>
-        <v>63360</v>
+        <v>158400</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="22">
+        <v>934</v>
+      </c>
+      <c r="C29" s="22">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="23">
-        <v>934</v>
-      </c>
-      <c r="C29" s="23">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="23">
+      <c r="B30" s="22">
         <v>138.89599999999999</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="22">
         <f>ROUND(PRODUCT(Tabella2[[#This Row],[Price]],12),0)</f>
         <v>1667</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="23">
+      <c r="A31" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="22">
         <v>51.54</v>
       </c>
-      <c r="C31" s="23">
+      <c r="C31" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],12,3)</f>
         <v>1855.44</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>58</v>
+      <c r="D31" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="23">
+      <c r="A32" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="22">
         <v>20</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23">
+      <c r="C32" s="22"/>
+      <c r="D32" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],30,3)</f>
         <v>1800</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],30,2)</f>
         <v>1200</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],30)</f>
         <v>600</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="23">
+      <c r="A33" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="22">
         <v>20</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23">
+      <c r="C33" s="22"/>
+      <c r="D33" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],30,3)</f>
         <v>1800</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],30,2)</f>
         <v>1200</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],30)</f>
         <v>600</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="23">
+      <c r="A34" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="22">
         <v>170</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23">
+      <c r="C34" s="22"/>
+      <c r="D34" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2,3)</f>
         <v>1020</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2,2)</f>
         <v>680</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2,1)</f>
         <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="23">
+      <c r="A35" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="22">
         <v>1000</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23">
+      <c r="C35" s="22"/>
+      <c r="D35" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2,3)</f>
         <v>6000</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2,2)</f>
         <v>4000</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2)</f>
         <v>2000</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="23">
+      <c r="A36" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="22">
         <v>245</v>
       </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23">
+      <c r="C36" s="22"/>
+      <c r="D36" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2,3)</f>
         <v>1470</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E36" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2,2)</f>
         <v>980</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="22">
         <f>PRODUCT(Tabella2[[#This Row],[Price]],2)</f>
         <v>490</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="23">
-        <v>4000</v>
-      </c>
-      <c r="C37" s="23">
-        <f>PRODUCT(Tabella2[[#This Row],[Price]],12)</f>
+      <c r="A37" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22">
         <v>48000</v>
+      </c>
+      <c r="D37" s="22">
+        <f>PRODUCT(Tabella2[[#This Row],[Total cost]],3/6)</f>
+        <v>24000</v>
+      </c>
+      <c r="E37" s="22">
+        <f>PRODUCT(Tabella2[[#This Row],[Total cost]],2/6)</f>
+        <v>16000</v>
+      </c>
+      <c r="F37" s="22">
+        <f>PRODUCT(Tabella2[[#This Row],[Total cost]],1/6)</f>
+        <v>8000</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1731,64 +1876,64 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="22">
+        <v>10</v>
+      </c>
+      <c r="C43" s="22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="23">
-        <v>10</v>
-      </c>
-      <c r="C43" s="23">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="23">
+      <c r="B44" s="22">
         <v>2.5</v>
       </c>
-      <c r="C44" s="23">
+      <c r="C44" s="22">
         <v>2000</v>
       </c>
-      <c r="D44" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" s="23" t="s">
-        <v>58</v>
+      <c r="D44" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="23">
+      <c r="A45" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="22">
         <v>474</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23">
+      <c r="C45" s="22"/>
+      <c r="D45" s="22">
         <f>PRODUCT(Tabella6[[#This Row],[Price]],0.05,12000)</f>
         <v>284400.00000000006</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E45" s="22">
         <f>PRODUCT(Tabella6[[#This Row],[Price]],0.05,24000)</f>
         <v>568800.00000000012</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="22">
         <f>PRODUCT(Tabella6[[#This Row],[Price]],0.05,36000)</f>
         <v>853200.00000000012</v>
       </c>
@@ -1803,7 +1948,7 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="59" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
   <tableParts count="5">
@@ -1818,168 +1963,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:T16"/>
+  <dimension ref="A2:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="95.88671875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" ht="28.2" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:2" ht="28.2" x14ac:dyDescent="0.5">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="21" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I3" t="s">
+      <c r="B16" s="20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="T8" s="21"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="21" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B23" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>70</v>
-      </c>
+      <c r="D23" s="26"/>
+      <c r="I23" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{527B1321-1F9F-4676-9636-E251E8D25623}"/>
-    <hyperlink ref="O8" r:id="rId2" xr:uid="{48C3DBBC-D077-4C57-9E21-BD5C4BA9C379}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{2FDF942B-1E38-4994-8F79-B50599473D11}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{FBB8B01A-CC7E-48F8-A189-AC3BFA7E6DA9}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{D46E2020-1624-41A3-840C-76CBE2E60ABB}"/>
-    <hyperlink ref="B12" r:id="rId6" location=":~:text=Affitti%20per%20studenti%3A%20il%20prezzo%20dipende%20dalla%20citt%C3%A0,-Secondo%20il%20centro&amp;text=Nella%20Capitale%2C%20infatti%2C%20per%20una,quinta%20posizione%20con%20447%20euro." xr:uid="{6B7DC9CD-989E-4460-A5D4-03CA0DDD6FCC}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{02E2B4CC-AD52-445C-8CA0-598F2897B67F}"/>
-    <hyperlink ref="B11" r:id="rId8" xr:uid="{F5FB9113-5952-48D6-A6A8-0E6045389D84}"/>
-    <hyperlink ref="B13" r:id="rId9" xr:uid="{FD6C4BEE-48BC-4195-9F15-7CF11A7B51E7}"/>
-    <hyperlink ref="B14" r:id="rId10" display="https://www.affissionitalia.com/categoria-prodotto/affissioni-campania/" xr:uid="{AD599595-5157-43DA-8CB9-0038393C145F}"/>
-    <hyperlink ref="B15" r:id="rId11" display="https://www.affissionitalia.com/categoria-prodotto/affissioni-lazio/affissioni-roma/" xr:uid="{E8AEEF6C-4A85-4E2C-99DD-ABB819383A1F}"/>
-    <hyperlink ref="B16" r:id="rId12" display="https://www.affissionitalia.com/categoria-prodotto/affissioni-lombardia/affissioni-milano-affissioni-lombardia/" xr:uid="{8C124C3D-9497-493A-AF07-04D458846537}"/>
-    <hyperlink ref="G8" r:id="rId13" xr:uid="{28ACAA9B-F0DC-4397-9080-29FFACFED15B}"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{407522EA-2750-4269-8BA0-F06214475D5F}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{4C4F0C6D-7218-42F6-AEB8-2D3874A26FC1}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{01FA4B59-4013-4FD2-8734-4250D0C55183}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{7CDF9A8D-44D2-41E4-87FB-6C93348EF86D}"/>
+    <hyperlink ref="B15" r:id="rId5" location=":~:text=Affitti%20per%20studenti%3A%20il%20prezzo%20dipende%20dalla%20citt%C3%A0,-Secondo%20il%20centro&amp;text=Nella%20Capitale%2C%20infatti%2C%20per%20una,quinta%20posizione%20con%20447%20euro." xr:uid="{14D7CC1F-442A-403B-946A-4B1ED9EC177A}"/>
+    <hyperlink ref="B12" r:id="rId6" xr:uid="{251C1E2B-9D86-4F41-BA2B-6D9EB87DD77B}"/>
+    <hyperlink ref="B14" r:id="rId7" xr:uid="{C98F3557-83DC-4CA5-9E7F-0F54D528B5A6}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{721A72E2-51BE-445C-896C-6240D27DD920}"/>
+    <hyperlink ref="B17" r:id="rId9" display="https://www.affissionitalia.com/categoria-prodotto/affissioni-campania/" xr:uid="{B5284C05-9617-428F-8ACB-9774FF3DED5F}"/>
+    <hyperlink ref="B18" r:id="rId10" display="https://www.affissionitalia.com/categoria-prodotto/affissioni-lazio/affissioni-roma/" xr:uid="{2FEB793A-5997-46B8-90DB-46695D71363E}"/>
+    <hyperlink ref="B19" r:id="rId11" display="https://www.affissionitalia.com/categoria-prodotto/affissioni-lombardia/affissioni-milano-affissioni-lombardia/" xr:uid="{FBD29D74-E3EB-45A8-BBF9-78980905B0D8}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId12"/>
+  <tableParts count="1">
+    <tablePart r:id="rId13"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>